<commit_message>
finishing analysis for 20190509
</commit_message>
<xml_diff>
--- a/code/processing/growth_curves_plate_reader/20190509_r1_chlor_dilution_test/20190509_plate_layout.xlsx
+++ b/code/processing/growth_curves_plate_reader/20190509_r1_chlor_dilution_test/20190509_plate_layout.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="15940" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="15940" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="strain" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,10 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="300" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="300" uniqueCount="77">
+  <si>
+    <t>blank</t>
+  </si>
   <si>
     <t>None</t>
   </si>
@@ -575,202 +578,202 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:J6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="G1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="H1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="I1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="J1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B2" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C2" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D2" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E2" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F2" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="G2" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="H2" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="I2" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="J2" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B3" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C3" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D3" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E3" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="F3" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="G3" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H3" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="I3" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="J3" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B4" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C4" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D4" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E4" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F4" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="G4" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="H4" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="I4" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="J4" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B5" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C5" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D5" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E5" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F5" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="G5" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="H5" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="I5" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="J5" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B6" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C6" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D6" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E6" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="F6" t="s">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="G6" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H6" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="I6" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="J6" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
   </sheetData>
@@ -782,202 +785,202 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I9" sqref="I9"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:J6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="G1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="H1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="I1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="J1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B2" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C2" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D2" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="E2" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="F2" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="G2" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="H2" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="I2" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="J2" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B3" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C3" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="D3" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="E3" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="F3" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="G3" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="H3" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="I3" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="J3" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B4" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C4" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D4" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="E4" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="F4" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="G4" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="H4" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="I4" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="J4" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B5" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="C5" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="D5" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="E5" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="F5" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="G5" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="H5" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="I5" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="J5" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B6" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="C6" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="D6" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="E6" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="F6" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="G6" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="H6" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="I6" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="J6" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
     </row>
   </sheetData>
@@ -997,194 +1000,194 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="I1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="J1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B2" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C2" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D2" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E2" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F2" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G2" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H2" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="I2" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="J2" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B3" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C3" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D3" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E3" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F3" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G3" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H3" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="I3" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="J3" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C4" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D4" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E4" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F4" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G4" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H4" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="I4" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="J4" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C5" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D5" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E5" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F5" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G5" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H5" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="I5" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="J5" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B6" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C6" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D6" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E6" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F6" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G6" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H6" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="I6" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="J6" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
   </sheetData>
@@ -1204,194 +1207,194 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D2" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E2" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F2" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G2" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H2" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I2" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J2" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C3" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D3" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E3" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F3" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G3" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H3" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I3" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J3" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C4" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D4" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E4" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F4" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G4" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H4" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I4" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J4" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B5" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C5" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D5" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E5" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F5" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G5" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H5" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I5" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J5" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B6" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C6" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D6" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E6" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F6" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G6" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H6" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I6" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J6" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
   </sheetData>
@@ -1411,194 +1414,194 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="F1" t="s">
+        <v>14</v>
+      </c>
+      <c r="G1" t="s">
+        <v>15</v>
+      </c>
+      <c r="H1" t="s">
         <v>13</v>
       </c>
-      <c r="G1" t="s">
-        <v>14</v>
-      </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>12</v>
       </c>
-      <c r="I1" t="s">
-        <v>11</v>
-      </c>
       <c r="J1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="F2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H2" t="s">
         <v>13</v>
       </c>
-      <c r="G2" t="s">
-        <v>14</v>
-      </c>
-      <c r="H2" t="s">
+      <c r="I2" t="s">
         <v>12</v>
       </c>
-      <c r="I2" t="s">
-        <v>11</v>
-      </c>
       <c r="J2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B3" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C3" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D3" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E3" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="F3" t="s">
+        <v>14</v>
+      </c>
+      <c r="G3" t="s">
+        <v>15</v>
+      </c>
+      <c r="H3" t="s">
         <v>13</v>
       </c>
-      <c r="G3" t="s">
-        <v>14</v>
-      </c>
-      <c r="H3" t="s">
+      <c r="I3" t="s">
         <v>12</v>
       </c>
-      <c r="I3" t="s">
-        <v>11</v>
-      </c>
       <c r="J3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B4" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C4" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="F4" t="s">
+        <v>14</v>
+      </c>
+      <c r="G4" t="s">
+        <v>15</v>
+      </c>
+      <c r="H4" t="s">
         <v>13</v>
       </c>
-      <c r="G4" t="s">
-        <v>14</v>
-      </c>
-      <c r="H4" t="s">
+      <c r="I4" t="s">
         <v>12</v>
       </c>
-      <c r="I4" t="s">
-        <v>11</v>
-      </c>
       <c r="J4" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B5" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C5" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D5" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E5" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="F5" t="s">
+        <v>14</v>
+      </c>
+      <c r="G5" t="s">
+        <v>15</v>
+      </c>
+      <c r="H5" t="s">
         <v>13</v>
       </c>
-      <c r="G5" t="s">
-        <v>14</v>
-      </c>
-      <c r="H5" t="s">
+      <c r="I5" t="s">
         <v>12</v>
       </c>
-      <c r="I5" t="s">
-        <v>11</v>
-      </c>
       <c r="J5" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C6" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D6" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E6" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="F6" t="s">
+        <v>14</v>
+      </c>
+      <c r="G6" t="s">
+        <v>15</v>
+      </c>
+      <c r="H6" t="s">
         <v>13</v>
       </c>
-      <c r="G6" t="s">
-        <v>14</v>
-      </c>
-      <c r="H6" t="s">
+      <c r="I6" t="s">
         <v>12</v>
       </c>
-      <c r="I6" t="s">
-        <v>11</v>
-      </c>
       <c r="J6" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>